<commit_message>
Creando excel de productos
</commit_message>
<xml_diff>
--- a/listado_productos.xlsx
+++ b/listado_productos.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\ventas_repuestos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="51">
   <si>
     <t>Producto 01</t>
   </si>
@@ -117,6 +112,66 @@
   </si>
   <si>
     <t>Producto 30</t>
+  </si>
+  <si>
+    <t>Producto 31</t>
+  </si>
+  <si>
+    <t>Producto 32</t>
+  </si>
+  <si>
+    <t>Producto 33</t>
+  </si>
+  <si>
+    <t>Producto 34</t>
+  </si>
+  <si>
+    <t>Producto 35</t>
+  </si>
+  <si>
+    <t>Producto 36</t>
+  </si>
+  <si>
+    <t>Producto 37</t>
+  </si>
+  <si>
+    <t>Producto 38</t>
+  </si>
+  <si>
+    <t>Producto 39</t>
+  </si>
+  <si>
+    <t>Producto 40</t>
+  </si>
+  <si>
+    <t>Producto 41</t>
+  </si>
+  <si>
+    <t>Producto 42</t>
+  </si>
+  <si>
+    <t>Producto 43</t>
+  </si>
+  <si>
+    <t>Producto 44</t>
+  </si>
+  <si>
+    <t>Producto 45</t>
+  </si>
+  <si>
+    <t>Producto 46</t>
+  </si>
+  <si>
+    <t>Producto 47</t>
+  </si>
+  <si>
+    <t>Producto 48</t>
+  </si>
+  <si>
+    <t>Producto 49</t>
+  </si>
+  <si>
+    <t>Producto 50</t>
   </si>
 </sst>
 </file>
@@ -214,7 +269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -249,7 +304,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -426,7 +481,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -434,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N30"/>
+      <selection activeCell="L30" sqref="L30:N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,6 +1817,886 @@
         <v>1</v>
       </c>
     </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1100911145</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>2</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>10</v>
+      </c>
+      <c r="N31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1100911146</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>10</v>
+      </c>
+      <c r="N32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1100911147</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="K33">
+        <v>2</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>10</v>
+      </c>
+      <c r="N33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1100911148</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>10</v>
+      </c>
+      <c r="N34" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1100911149</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>2</v>
+      </c>
+      <c r="K35">
+        <v>2</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>10</v>
+      </c>
+      <c r="N35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1100911150</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36">
+        <v>2</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>2</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>10</v>
+      </c>
+      <c r="N36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1100911151</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>10</v>
+      </c>
+      <c r="N37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1100911152</v>
+      </c>
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38">
+        <v>2</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>10</v>
+      </c>
+      <c r="N38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1100911153</v>
+      </c>
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>10</v>
+      </c>
+      <c r="N39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1100911154</v>
+      </c>
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>2</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>2</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>10</v>
+      </c>
+      <c r="N40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1100911155</v>
+      </c>
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41">
+        <v>2</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>2</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>10</v>
+      </c>
+      <c r="N41" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1100911156</v>
+      </c>
+      <c r="B42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>2</v>
+      </c>
+      <c r="I42">
+        <v>2</v>
+      </c>
+      <c r="J42">
+        <v>2</v>
+      </c>
+      <c r="K42">
+        <v>2</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>10</v>
+      </c>
+      <c r="N42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1100911157</v>
+      </c>
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>2</v>
+      </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>2</v>
+      </c>
+      <c r="K43">
+        <v>2</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>10</v>
+      </c>
+      <c r="N43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1100911158</v>
+      </c>
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>2</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <v>10</v>
+      </c>
+      <c r="N44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1100911159</v>
+      </c>
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>2</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>10</v>
+      </c>
+      <c r="N45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1100911160</v>
+      </c>
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>2</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>2</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="M46">
+        <v>10</v>
+      </c>
+      <c r="N46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1100911161</v>
+      </c>
+      <c r="B47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>2</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>2</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47">
+        <v>10</v>
+      </c>
+      <c r="N47" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1100911162</v>
+      </c>
+      <c r="B48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>2</v>
+      </c>
+      <c r="H48">
+        <v>2</v>
+      </c>
+      <c r="I48">
+        <v>2</v>
+      </c>
+      <c r="J48">
+        <v>2</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48">
+        <v>10</v>
+      </c>
+      <c r="N48" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1100911163</v>
+      </c>
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49">
+        <v>2</v>
+      </c>
+      <c r="H49">
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>2</v>
+      </c>
+      <c r="K49">
+        <v>2</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <v>10</v>
+      </c>
+      <c r="N49" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1100911164</v>
+      </c>
+      <c r="B50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50">
+        <v>2</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>2</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <v>10</v>
+      </c>
+      <c r="N50" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>